<commit_message>
task 1 of day-4 has been completed with goal seek concept
</commit_message>
<xml_diff>
--- a/European_Coaching/day_2/excel/task-2.xlsx
+++ b/European_Coaching/day_2/excel/task-2.xlsx
@@ -144,10 +144,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,20 +463,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -528,35 +528,35 @@
       </c>
       <c r="E4">
         <f t="shared" ref="E4:J17" ca="1" si="0">RANDBETWEEN(39,89)</f>
+        <v>74</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
         <v>68</v>
       </c>
-      <c r="F4">
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="J4">
         <f t="shared" ca="1" si="0"/>
         <v>70</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>81</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ca="1" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I4">
-        <f t="shared" ca="1" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ca="1" si="0"/>
-        <v>51</v>
       </c>
       <c r="K4">
         <f ca="1">SUM(E4:J4)</f>
-        <v>355</v>
+        <v>434</v>
       </c>
       <c r="L4">
         <f ca="1">SUM(K4*100/600)</f>
-        <v>59.166666666666664</v>
+        <v>72.333333333333329</v>
       </c>
       <c r="M4" t="str">
         <f ca="1">IF(K4&gt;299,"1st division",IF(K4&gt;224,"2nd division",IF(K4&gt;164,"3rd division",IF(K4&lt;165,"fail"))))</f>
@@ -575,38 +575,38 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="J5">
         <f ca="1">RANDBETWEEN(39,89)</f>
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K17" ca="1" si="1">SUM(E5:J5)</f>
-        <v>362</v>
+        <v>420</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L18" ca="1" si="2">SUM(K5*100/600)</f>
-        <v>60.333333333333336</v>
+        <f t="shared" ref="L5:L17" ca="1" si="2">SUM(K5*100/600)</f>
+        <v>70</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" ref="M5:M19" ca="1" si="3">IF(K5&gt;299,"1st division",IF(K5&gt;224,"2nd division",IF(K5&gt;164,"3rd division",IF(K5&lt;165,"fail"))))</f>
+        <f t="shared" ref="M5:M17" ca="1" si="3">IF(K5&gt;299,"1st division",IF(K5&gt;224,"2nd division",IF(K5&gt;164,"3rd division",IF(K5&lt;165,"fail"))))</f>
         <v>1st division</v>
       </c>
     </row>
@@ -622,19 +622,19 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
@@ -642,15 +642,15 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>359</v>
+        <v>428</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="2"/>
-        <v>59.833333333333336</v>
+        <v>71.333333333333329</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -669,35 +669,35 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
         <v>82</v>
       </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="0"/>
-        <v>46</v>
-      </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="1"/>
-        <v>345</v>
+        <v>395</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="2"/>
-        <v>57.5</v>
+        <v>65.833333333333329</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -716,35 +716,35 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="1"/>
-        <v>374</v>
+        <v>407</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="2"/>
-        <v>62.333333333333336</v>
+        <v>67.833333333333329</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -763,35 +763,35 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="1"/>
-        <v>445</v>
+        <v>389</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="2"/>
-        <v>74.166666666666671</v>
+        <v>64.833333333333329</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -810,23 +810,23 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
@@ -834,11 +834,11 @@
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="1"/>
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="2"/>
-        <v>60.333333333333336</v>
+        <v>61.166666666666664</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -857,35 +857,35 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="1"/>
-        <v>344</v>
+        <v>368</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="2"/>
-        <v>57.333333333333336</v>
+        <v>61.333333333333336</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -904,35 +904,35 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="0"/>
         <v>63</v>
       </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="0"/>
-        <v>81</v>
-      </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="1"/>
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="2"/>
-        <v>64.166666666666671</v>
+        <v>60.5</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -951,35 +951,35 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <f t="shared" ca="1" si="0"/>
         <v>47</v>
       </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ca="1" si="0"/>
-        <v>69</v>
-      </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="1"/>
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <v>57.5</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -998,35 +998,35 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="1"/>
-        <v>338</v>
+        <v>367</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="2"/>
-        <v>56.333333333333336</v>
+        <v>61.166666666666664</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1045,35 +1045,35 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="1"/>
-        <v>429</v>
+        <v>355</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="2"/>
-        <v>71.5</v>
+        <v>59.166666666666664</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1092,35 +1092,35 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
-      <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="G16">
-        <f t="shared" ca="1" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ca="1" si="0"/>
-        <v>54</v>
-      </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="1"/>
-        <v>351</v>
+        <v>319</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="2"/>
-        <v>58.5</v>
+        <v>53.166666666666664</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1139,35 +1139,35 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>341</v>
+        <v>370</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="2"/>
-        <v>56.833333333333336</v>
+        <v>61.666666666666664</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1197,20 +1197,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1262,35 +1262,35 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:I16" ca="1" si="0">RANDBETWEEN(39,89)</f>
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
         <v>65</v>
       </c>
-      <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>73</v>
-      </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="J3">
         <f ca="1">SUM(D3:I3)</f>
-        <v>417</v>
+        <v>348</v>
       </c>
       <c r="K3">
         <f ca="1">SUM(J3*100/600)</f>
-        <v>69.5</v>
+        <v>58</v>
       </c>
       <c r="L3" t="str">
         <f ca="1">IF(J3&gt;299,"1st division",IF(J3&gt;224,"2nd division",IF(J3&gt;164,"3rd division",IF(J3&lt;165,"fail"))))</f>
@@ -1309,35 +1309,35 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J16" ca="1" si="1">SUM(D4:I4)</f>
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K16" ca="1" si="2">SUM(J4*100/600)</f>
-        <v>61.333333333333336</v>
+        <v>59.166666666666664</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ref="L4:L16" ca="1" si="3">IF(J4&gt;299,"1st division",IF(J4&gt;224,"2nd division",IF(J4&gt;164,"3rd division",IF(J4&lt;165,"fail"))))</f>
@@ -1356,19 +1356,19 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
@@ -1376,15 +1376,15 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>348</v>
+        <v>313</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="2"/>
-        <v>58</v>
+        <v>52.166666666666664</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1403,35 +1403,35 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="0"/>
         <v>70</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="0"/>
-        <v>81</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ca="1" si="0"/>
-        <v>67</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>402</v>
+        <v>421</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="2"/>
-        <v>67</v>
+        <v>70.166666666666671</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1450,35 +1450,35 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>386</v>
+        <v>431</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="2"/>
-        <v>64.333333333333329</v>
+        <v>71.833333333333329</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1497,35 +1497,35 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>417</v>
+        <v>367</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="2"/>
-        <v>69.5</v>
+        <v>61.166666666666664</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1544,35 +1544,35 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="1"/>
-        <v>364</v>
+        <v>317</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="2"/>
-        <v>60.666666666666664</v>
+        <v>52.833333333333336</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1591,35 +1591,35 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="0"/>
         <v>76</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ca="1" si="0"/>
-        <v>74</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="1"/>
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="2"/>
-        <v>60.5</v>
+        <v>73.833333333333329</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1638,35 +1638,35 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="1"/>
-        <v>340</v>
+        <v>412</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="2"/>
-        <v>56.666666666666664</v>
+        <v>68.666666666666671</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1685,35 +1685,35 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="1"/>
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="2"/>
-        <v>62.666666666666664</v>
+        <v>63.166666666666664</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1736,31 +1736,31 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="1"/>
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="2"/>
-        <v>57.166666666666664</v>
+        <v>56.166666666666664</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1779,35 +1779,35 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="1"/>
-        <v>399</v>
+        <v>345</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="2"/>
-        <v>66.5</v>
+        <v>57.5</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1826,35 +1826,35 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="1"/>
-        <v>429</v>
+        <v>336</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="2"/>
-        <v>71.5</v>
+        <v>56</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1873,35 +1873,35 @@
       </c>
       <c r="D16">
         <f ca="1">RANDBETWEEN(39,89)</f>
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="1"/>
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="2"/>
-        <v>60.833333333333336</v>
+        <v>65</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1939,767 +1939,767 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>3</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>6</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>7</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>8</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>9</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>10</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>11</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>12</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>13</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>1001</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1002</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1003</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>1004</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>1005</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>1006</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>1007</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>1008</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>1009</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>1010</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>1011</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>1012</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>1013</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>1014</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>70</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>49</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>87</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>45</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>54</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>71</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>86</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>76</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>40</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <v>83</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <v>84</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <v>55</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <v>40</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>80</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>75</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>64</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>53</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>88</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>86</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>66</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>79</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>46</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <v>48</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <v>58</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <v>76</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <v>39</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>48</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>60</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>78</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>89</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>41</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>71</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>67</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>41</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>51</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <v>55</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>62</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1">
         <v>45</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="1">
         <v>64</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="1">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>73</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>58</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>84</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>71</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>86</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>65</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>67</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>73</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>82</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <v>80</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <v>42</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="1">
         <v>73</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="1">
         <v>59</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="1">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>54</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>40</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>61</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>49</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>86</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>61</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>42</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>67</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="1">
         <v>53</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="1">
         <v>56</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="1">
         <v>58</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="1">
         <v>40</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="1">
         <v>65</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="1">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>85</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>87</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>79</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>41</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>83</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>48</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>82</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>54</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>52</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="1">
         <v>56</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="1">
         <v>58</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="1">
         <v>48</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="1">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>410</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>369</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>453</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>373</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>396</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>437</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>376</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>418</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>326</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <v>374</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <v>360</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <v>347</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="1">
         <v>315</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="1">
         <v>367</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>68.333333333333329</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>61.5</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>75.5</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>62.166666666666664</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>66</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>72.833333333333329</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>62.666666666666664</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>69.666666666666671</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>54.333333333333336</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <v>62.333333333333336</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="1">
         <v>60</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1">
         <v>57.833333333333336</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="1">
         <v>52.5</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="1">
         <v>61.166666666666664</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P14" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>2</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="2" t="str">
+      <c r="C22" s="1" t="str">
         <f>HLOOKUP($C$21,$B$2:$P$14,A22,0)</f>
         <v>shoan</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>3</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="str">
+      <c r="C23" s="1" t="str">
         <f t="shared" ref="C23:C33" si="0">HLOOKUP($C$21,$B$2:$P$14,A23,0)</f>
         <v>XII</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <f t="shared" si="0"/>
         <v>1003</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>5</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>6</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>7</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>8</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>9</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>10</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>11</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <f t="shared" si="0"/>
         <v>453</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>12</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <f t="shared" si="0"/>
         <v>75.5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>13</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="2" t="str">
+      <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>1st division</v>
       </c>

</xml_diff>